<commit_message>
Adding Data Provider to adding new customer
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/TestData.xlsx
+++ b/src/main/resources/excel/TestData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataDrivenTestingHub\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AA4647B-19B8-4B7C-84DC-C2EAB455A24C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688343D1-D62F-4F3C-8BCC-A4874872B1BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2496" yWindow="3396" windowWidth="19176" windowHeight="8964" xr2:uid="{266132B8-4321-491B-A948-1E9EED1C36DE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CustomerData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,10 +33,47 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>PostCode</t>
+  </si>
+  <si>
+    <t>Meenakshi</t>
+  </si>
+  <si>
+    <t>Rana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vamika </t>
+  </si>
+  <si>
+    <t>Dogra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pardeep </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -64,8 +101,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,12 +418,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{071D7CB6-F72E-4C1B-9572-F0BC85467973}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>